<commit_message>
refactor , adding more variables
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1112,9 +1112,67 @@
         <v>28.00%</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>pumas unam</v>
+      </c>
+      <c r="B26" t="str">
+        <v>3</v>
+      </c>
+      <c r="C26" t="str">
+        <v>2</v>
+      </c>
+      <c r="D26" t="str">
+        <v>1</v>
+      </c>
+      <c r="E26" t="str">
+        <v>1</v>
+      </c>
+      <c r="F26" t="str">
+        <v>66.67%</v>
+      </c>
+      <c r="G26" t="str">
+        <v>66.67%</v>
+      </c>
+      <c r="H26" t="str">
+        <v>66.67%</v>
+      </c>
+      <c r="I26" t="str">
+        <v>50.00%</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>pachuca</v>
+      </c>
+      <c r="B27" t="str">
+        <v>3</v>
+      </c>
+      <c r="C27" t="str">
+        <v>1</v>
+      </c>
+      <c r="D27" t="str">
+        <v>1</v>
+      </c>
+      <c r="E27" t="str">
+        <v>1</v>
+      </c>
+      <c r="F27" t="str">
+        <v>33.33%</v>
+      </c>
+      <c r="G27" t="str">
+        <v>33.33%</v>
+      </c>
+      <c r="H27" t="str">
+        <v>33.33%</v>
+      </c>
+      <c r="I27" t="str">
+        <v>50.00%</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
predictions filled some columns
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -443,42 +443,45 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>45499.66148540509</v>
+        <v>45499.675166099536</v>
       </c>
       <c r="B2" t="str">
-        <v>isd</v>
+        <v>atlanta braves</v>
       </c>
       <c r="E2" t="str">
         <v>1</v>
       </c>
       <c r="G2">
-        <v>33.33333333333333</v>
+        <v>54</v>
       </c>
       <c r="H2">
-        <v>0.36</v>
+        <v>0.5421818181818182</v>
+      </c>
+      <c r="K2">
+        <v>8.51063829787234</v>
       </c>
       <c r="L2">
-        <v>26.874023251381736</v>
+        <v>3.451931103924922</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>45499.66148540509</v>
+        <v>45499.675166099536</v>
       </c>
       <c r="B3" t="str">
-        <v>sdasda</v>
+        <v>mets</v>
       </c>
       <c r="E3" t="str">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>41.66666666666667</v>
+        <v>53</v>
       </c>
       <c r="H3">
-        <v>0.4455555555555556</v>
+        <v>0.4270909090909091</v>
       </c>
       <c r="L3">
-        <v>33.590157338585016</v>
+        <v>3.3835593431939115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>